<commit_message>
[Add] excel file export related programs
</commit_message>
<xml_diff>
--- a/storage/app/Excel_format/Template_EngineerCareer.xlsx
+++ b/storage/app/Excel_format/Template_EngineerCareer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\engr_info_app\storage\app\Excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB53567-5D11-4FB9-AF73-E3EC172EE2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F413A9-0471-4B64-9C7B-D5213B52527F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,11 +25,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>名前（漢字）</t>
-    <rPh sb="0" eb="2">
-      <t>ナマエ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>資格</t>
+    <rPh sb="0" eb="2">
+      <t>シカク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>経験年数</t>
+    <rPh sb="0" eb="2">
+      <t>ケイケン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ネンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最寄り駅</t>
+    <rPh sb="0" eb="2">
+      <t>モヨ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>エキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開発環境</t>
+    <rPh sb="0" eb="2">
+      <t>カイハツ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カンキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プログラミング言語</t>
+    <rPh sb="7" eb="9">
+      <t>ゲンゴ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>氏名（漢字）</t>
+    <rPh sb="0" eb="2">
+      <t>シメイ</t>
     </rPh>
     <rPh sb="3" eb="5">
       <t>カンジ</t>
@@ -37,9 +85,104 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>名前（カナ）</t>
-    <rPh sb="0" eb="2">
-      <t>ナマエ</t>
+    <t>氏名（カナ）</t>
+    <rPh sb="0" eb="2">
+      <t>シメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エンジニア基本情報</t>
+    <rPh sb="5" eb="9">
+      <t>キホンジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>システムエンジニア経歴書</t>
+    <rPh sb="9" eb="12">
+      <t>ケイレキショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エンジニア経歴（実績）情報</t>
+    <rPh sb="5" eb="7">
+      <t>ケイレキ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ジッセキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロジェクト概要</t>
+    <rPh sb="6" eb="8">
+      <t>ガイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実施タスク</t>
+    <rPh sb="0" eb="2">
+      <t>ジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実績No</t>
+    <rPh sb="0" eb="2">
+      <t>ジッセキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開発環境
+(サーバ、PG言語など）</t>
+    <rPh sb="0" eb="2">
+      <t>カイハツ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ゲンゴ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>役割
+（職務）</t>
+    <rPh sb="0" eb="2">
+      <t>ヤクワリ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ショクム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>参加期間
+（from）</t>
+    <rPh sb="0" eb="2">
+      <t>サンカ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>参加期間
+（to）</t>
+    <rPh sb="0" eb="2">
+      <t>サンカ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キカン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -48,7 +191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,16 +206,57 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF6600"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -80,18 +264,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -366,23 +616,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.25" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.4140625" customWidth="1"/>
+    <col min="3" max="3" width="17.9140625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="10.58203125" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
+    <row r="1" spans="1:9" ht="32.5">
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="26.5">
+      <c r="B2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="1"/>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="31.5" customHeight="1">
+      <c r="B12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="36">
+      <c r="B13" s="1"/>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="38" customHeight="1">
+      <c r="B14" s="1"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="38" customHeight="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" ht="38" customHeight="1">
+      <c r="B16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" ht="38" customHeight="1">
+      <c r="B17" s="1"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9" ht="38" customHeight="1">
+      <c r="B18" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:9" ht="38" customHeight="1">
+      <c r="B19" s="1"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>